<commit_message>
Added support for multi-row execution.
</commit_message>
<xml_diff>
--- a/examples/example-data.xlsx
+++ b/examples/example-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ird/dev/iandinwoodie/pdfpop/tests/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ird/dev/iandinwoodie/pdfpop/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D14029-05C4-B34F-BDC8-54E642A6B7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F61FA5-89E1-8D43-BC7F-3B5C1C483FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2740" yWindow="1780" windowWidth="28040" windowHeight="17440" xr2:uid="{2E22BE47-51BF-5949-B04C-74FB168D666A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Email</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Doe</t>
   </si>
   <si>
-    <t>john.doe@fake.com</t>
-  </si>
-  <si>
     <t>999-999-9999</t>
   </si>
   <si>
@@ -98,6 +95,30 @@
   </si>
   <si>
     <t>Extend hours,Lower fees,Add more space</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>john.smith@fake.com</t>
+  </si>
+  <si>
+    <t>jane.doe@fake.com</t>
+  </si>
+  <si>
+    <t>123-123-1234</t>
+  </si>
+  <si>
+    <t>ACC124</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Music is too loud.</t>
   </si>
 </sst>
 </file>
@@ -453,17 +474,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D362D0B9-1B01-0944-B9A7-B547E2ED724E}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
   </cols>
@@ -485,22 +507,22 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" t="s">
         <v>4</v>
@@ -511,34 +533,69 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1">
         <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1">
+        <v>34.99</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>